<commit_message>
Data Analytics by Bokeh
</commit_message>
<xml_diff>
--- a/Data analytics with python/problems-1/PROBLEM 1.xlsx
+++ b/Data analytics with python/problems-1/PROBLEM 1.xlsx
@@ -994,8 +994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D36" workbookViewId="0">
-      <selection activeCell="L43" sqref="L43"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
small changes for better code practice
</commit_message>
<xml_diff>
--- a/Data analytics with python/problems-1/PROBLEM 1.xlsx
+++ b/Data analytics with python/problems-1/PROBLEM 1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PYTHON projects\Problems\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\Tableau Documentation\Data analytics with python\problems-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -994,8 +994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2303,47 +2303,53 @@
     </row>
     <row r="44" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
+      <c r="B44" s="5"/>
       <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="5"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
+      <c r="I44" s="2">
+        <v>1</v>
+      </c>
       <c r="J44" s="2"/>
     </row>
     <row r="45" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
+      <c r="B45" s="5"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="5"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
+      <c r="I45" s="2">
+        <v>1</v>
+      </c>
       <c r="J45" s="2"/>
     </row>
     <row r="46" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
+      <c r="B46" s="5"/>
       <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="5"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
+      <c r="I46" s="2">
+        <v>1</v>
+      </c>
       <c r="J46" s="2"/>
     </row>
     <row r="47" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
+      <c r="B47" s="5"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="5"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>

</xml_diff>